<commit_message>
fix(gui): Refactor layout and style adjustments for better usability
- **EmailBotGuiC1**:
  - Removed fixed height for `_input_frame` to allow dynamic resizing.
  - Adjusted dropdown menu minimum widths for consistency and responsiveness.
  - Refactored dropdown container layout for better alignment and removed redundant code.

- **EmailBodyC1**:
  - Removed unnecessary minimum height for the email body widget.
  - Improved character typing event filter handling for enhanced functionality.

- **VariableLister**:
  - Simplified layout spacing and removed obsolete styles for compactness.
  - Changed button background color to `lightyellow` for better visual distinction.

- **FileSelector and FolderSelector**:
  - Updated layouts to include dynamic alignment for better responsiveness.
  - Refactored and cleaned up unused or commented-out style definitions.

- **Tests**: Updated `sample data file dynamic.xlsx`.
</commit_message>
<xml_diff>
--- a/tests/files/sample data file dynamic.xlsx
+++ b/tests/files/sample data file dynamic.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -67,6 +67,81 @@
   </si>
   <si>
     <t>Attachments</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -456,10 +531,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:CT5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="BD1" sqref="BD1:CT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +545,7 @@
     <col min="4" max="4" width="25.109375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:98" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +558,154 @@
       <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="4"/>
+      <c r="BE1" s="4"/>
+      <c r="BF1" s="4"/>
+      <c r="BG1" s="4"/>
+      <c r="BH1" s="4"/>
+      <c r="BI1" s="4"/>
+      <c r="BJ1" s="4"/>
+      <c r="BK1" s="4"/>
+      <c r="BL1" s="4"/>
+      <c r="BM1" s="4"/>
+      <c r="BN1" s="4"/>
+      <c r="BO1" s="4"/>
+      <c r="BP1" s="4"/>
+      <c r="BQ1" s="4"/>
+      <c r="BR1" s="4"/>
+      <c r="BS1" s="4"/>
+      <c r="BT1" s="4"/>
+      <c r="BU1" s="4"/>
+      <c r="BV1" s="4"/>
+      <c r="BW1" s="4"/>
+      <c r="BX1" s="4"/>
+      <c r="BY1" s="4"/>
+      <c r="BZ1" s="4"/>
+      <c r="CA1" s="4"/>
+      <c r="CB1" s="4"/>
+      <c r="CC1" s="4"/>
+      <c r="CD1" s="4"/>
+      <c r="CE1" s="4"/>
+      <c r="CF1" s="4"/>
+      <c r="CG1" s="4"/>
+      <c r="CH1" s="4"/>
+      <c r="CI1" s="4"/>
+      <c r="CJ1" s="4"/>
+      <c r="CK1" s="4"/>
+      <c r="CL1" s="4"/>
+      <c r="CM1" s="4"/>
+      <c r="CN1" s="4"/>
+      <c r="CO1" s="4"/>
+      <c r="CP1" s="4"/>
+      <c r="CQ1" s="4"/>
+      <c r="CR1" s="4"/>
+      <c r="CS1" s="4"/>
+      <c r="CT1" s="4"/>
     </row>
-    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:98" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -498,7 +719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:98" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -512,7 +733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:98" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -526,7 +747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:98" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5"/>

</xml_diff>